<commit_message>
1.Sample tests added 2.Fixed existing framework issues
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ServiceTestData.xlsx
+++ b/src/main/resources/data/ServiceTestData.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\308211\Desktop\Project Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhishekgummalla/IdeaProjects/ScaleServiceAutomation/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988D876D-5BDA-584C-B926-B52D4AD620C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16820" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,16 +25,121 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>TestData</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="36">
+  <si>
+    <t>SC_ID</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Company_001</t>
+  </si>
+  <si>
+    <t>Company_002</t>
+  </si>
+  <si>
+    <t>Company_003</t>
+  </si>
+  <si>
+    <t>Company_004</t>
+  </si>
+  <si>
+    <t>Company_005</t>
+  </si>
+  <si>
+    <t>Company_006</t>
+  </si>
+  <si>
+    <t>Company_007</t>
+  </si>
+  <si>
+    <t>/services/ChartWService.asmx/GetPrices</t>
+  </si>
+  <si>
+    <t>Check Price for</t>
+  </si>
+  <si>
+    <t>sampleTime</t>
+  </si>
+  <si>
+    <t>1d</t>
+  </si>
+  <si>
+    <t>sampleTimeFrame</t>
+  </si>
+  <si>
+    <t>3m</t>
+  </si>
+  <si>
+    <t>requestedDataSetType</t>
+  </si>
+  <si>
+    <t>ohlc</t>
+  </si>
+  <si>
+    <t>chartPriceType</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>III.LD</t>
+  </si>
+  <si>
+    <t>ABF.LD</t>
+  </si>
+  <si>
+    <t>ADM.LD</t>
+  </si>
+  <si>
+    <t>AAL.LD</t>
+  </si>
+  <si>
+    <t>ANTO.LD</t>
+  </si>
+  <si>
+    <t>AHT.LD</t>
+  </si>
+  <si>
+    <t>AZN.LD</t>
+  </si>
+  <si>
+    <t>content-Type</t>
+  </si>
+  <si>
+    <t>application/json; charset=UTF-8</t>
+  </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>https://charts.londonstockexchange.com</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>charts.londonstockexchange.com</t>
+  </si>
+  <si>
+    <t>EndPoint</t>
+  </si>
+  <si>
+    <t>ExpectedStatus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -41,16 +147,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -58,12 +193,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -343,21 +517,332 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="A1:C6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" customWidth="1"/>
+    <col min="3" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" customWidth="1"/>
+    <col min="12" max="12" width="51.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="1:12" ht="38" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>

</xml_diff>